<commit_message>
Added graphics output options, clarified convolution matrix
RCWA_process can now output a struct with all the data used in the figures.
conv_mat code now better reflects the RCWA theory, added support for matrices smaller than 2x # harmonics using zero padding
</commit_message>
<xml_diff>
--- a/input/layers.xlsx
+++ b/input/layers.xlsx
@@ -155,10 +155,10 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -218,19 +218,19 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>